<commit_message>
just continent zoom feature missing on map
</commit_message>
<xml_diff>
--- a/armenian_diaspora/shiny_app/data/processed_data.xlsx
+++ b/armenian_diaspora/shiny_app/data/processed_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/byronking/whatcheer_posts/armenian_diaspora/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/byronking/whatcheer_posts/armenian_diaspora/shiny_app/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182A5418-2418-9D45-8BD5-64F404A600DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39D60B9-992C-E547-AA55-7D0FF90FD5B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1759" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1741" uniqueCount="359">
   <si>
     <t>area</t>
   </si>
@@ -881,12 +881,6 @@
     <t>50.4500336</t>
   </si>
   <si>
-    <t>31.9771019</t>
-  </si>
-  <si>
-    <t>33.9597677</t>
-  </si>
-  <si>
     <t>49.9902794</t>
   </si>
   <si>
@@ -929,9 +923,6 @@
     <t>54.7066422</t>
   </si>
   <si>
-    <t>28.0836269</t>
-  </si>
-  <si>
     <t>42.1418541</t>
   </si>
   <si>
@@ -1058,12 +1049,6 @@
     <t>30.5241361</t>
   </si>
   <si>
-    <t>-91.336504</t>
-  </si>
-  <si>
-    <t>-83.376398</t>
-  </si>
-  <si>
     <t>36.2303893</t>
   </si>
   <si>
@@ -1104,9 +1089,6 @@
   </si>
   <si>
     <t>20.5105166</t>
-  </si>
-  <si>
-    <t>-80.6081089</t>
   </si>
   <si>
     <t>24.7499297</t>
@@ -1530,23 +1512,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F76" workbookViewId="0">
-      <selection activeCell="J95" sqref="J95"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="K75" sqref="K75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.1640625" customWidth="1"/>
-    <col min="6" max="6" width="164" customWidth="1"/>
-    <col min="7" max="7" width="10.5" customWidth="1"/>
-    <col min="8" max="8" width="10.1640625" customWidth="1"/>
-    <col min="9" max="9" width="12.83203125" customWidth="1"/>
-    <col min="10" max="10" width="13" customWidth="1"/>
-    <col min="11" max="12" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="30.1640625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="164" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1640625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="12.83203125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
@@ -1636,7 +1618,7 @@
         <v>248</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -1674,7 +1656,7 @@
         <v>247</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -1712,7 +1694,7 @@
         <v>248</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -1750,7 +1732,7 @@
         <v>249</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -1788,7 +1770,7 @@
         <v>250</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -1826,7 +1808,7 @@
         <v>251</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -1902,7 +1884,7 @@
         <v>252</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -1946,7 +1928,7 @@
         <v>253</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -2173,8 +2155,8 @@
       <c r="I16" t="s">
         <v>219</v>
       </c>
-      <c r="J16" t="s">
-        <v>239</v>
+      <c r="J16" s="5">
+        <v>250000</v>
       </c>
       <c r="K16" t="s">
         <v>239</v>
@@ -2186,7 +2168,7 @@
         <v>254</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
@@ -2211,8 +2193,8 @@
       <c r="I17" t="s">
         <v>220</v>
       </c>
-      <c r="J17" t="s">
-        <v>176</v>
+      <c r="J17" s="5">
+        <v>25000</v>
       </c>
       <c r="K17" t="s">
         <v>103</v>
@@ -2224,7 +2206,7 @@
         <v>254</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
@@ -2262,7 +2244,7 @@
         <v>255</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
@@ -2300,7 +2282,7 @@
         <v>256</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -2338,7 +2320,7 @@
         <v>257</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
@@ -2376,7 +2358,7 @@
         <v>258</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
@@ -2420,7 +2402,7 @@
         <v>259</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
@@ -2458,7 +2440,7 @@
         <v>259</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
@@ -2534,7 +2516,7 @@
         <v>260</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
@@ -2578,7 +2560,7 @@
         <v>40.712800000000001</v>
       </c>
       <c r="N26" s="1">
-        <v>74.006</v>
+        <v>-74.006</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
@@ -2616,7 +2598,7 @@
         <v>40.728200000000001</v>
       </c>
       <c r="N27" s="1">
-        <v>73.794899999999998</v>
+        <v>-73.794899999999998</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
@@ -2654,7 +2636,7 @@
         <v>261</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
@@ -2698,7 +2680,7 @@
         <v>262</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
@@ -2736,7 +2718,7 @@
         <v>263</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
@@ -2774,7 +2756,7 @@
         <v>264</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
@@ -2812,7 +2794,7 @@
         <v>265</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
@@ -2850,7 +2832,7 @@
         <v>266</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
@@ -2938,7 +2920,7 @@
         <v>42.360100000000003</v>
       </c>
       <c r="N35" s="1">
-        <v>71.058899999999994</v>
+        <v>-71.058899999999994</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
@@ -2976,7 +2958,7 @@
         <v>42.370899999999999</v>
       </c>
       <c r="N36" s="2">
-        <v>71.1828</v>
+        <v>-71.1828</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
@@ -3014,7 +2996,7 @@
         <v>42.395600000000002</v>
       </c>
       <c r="N37" s="2">
-        <v>71.177599999999998</v>
+        <v>-71.177599999999998</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
@@ -3052,7 +3034,7 @@
         <v>42.3765</v>
       </c>
       <c r="N38" s="2">
-        <v>71.235600000000005</v>
+        <v>-71.235600000000005</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
@@ -3096,7 +3078,7 @@
         <v>267</v>
       </c>
       <c r="N39" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
@@ -3134,7 +3116,7 @@
         <v>268</v>
       </c>
       <c r="N40" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
@@ -3174,11 +3156,11 @@
       <c r="L41" t="s">
         <v>103</v>
       </c>
-      <c r="M41" s="1" t="s">
-        <v>268</v>
-      </c>
-      <c r="N41" s="1" t="s">
-        <v>327</v>
+      <c r="M41" s="1">
+        <v>37.774900000000002</v>
+      </c>
+      <c r="N41" s="1">
+        <v>-122.4194</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
@@ -3222,7 +3204,7 @@
         <v>269</v>
       </c>
       <c r="N42" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.2">
@@ -3310,7 +3292,7 @@
         <v>42.331400000000002</v>
       </c>
       <c r="N44" s="2">
-        <v>83.0458</v>
+        <v>-83.0458</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
@@ -3354,7 +3336,7 @@
         <v>41.878100000000003</v>
       </c>
       <c r="N45" s="2">
-        <v>87.629800000000003</v>
+        <v>-87.629800000000003</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
@@ -3392,7 +3374,7 @@
         <v>270</v>
       </c>
       <c r="N46" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
@@ -3430,7 +3412,7 @@
         <v>271</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
@@ -3474,7 +3456,7 @@
         <v>271</v>
       </c>
       <c r="N48" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
@@ -3518,7 +3500,7 @@
         <v>272</v>
       </c>
       <c r="N49" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.2">
@@ -3562,7 +3544,7 @@
         <v>273</v>
       </c>
       <c r="N50" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.2">
@@ -3606,7 +3588,7 @@
         <v>274</v>
       </c>
       <c r="N51" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.2">
@@ -3690,11 +3672,11 @@
       <c r="L53" t="s">
         <v>103</v>
       </c>
-      <c r="M53" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="N53" s="1" t="s">
-        <v>334</v>
+      <c r="M53" s="1">
+        <v>45.357315</v>
+      </c>
+      <c r="N53" s="1">
+        <v>36.468291999999998</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.2">
@@ -3728,11 +3710,11 @@
       <c r="L54" t="s">
         <v>103</v>
       </c>
-      <c r="M54" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="N54" s="1" t="s">
-        <v>335</v>
+      <c r="M54" s="1">
+        <v>37.995538000000003</v>
+      </c>
+      <c r="N54" s="1">
+        <v>23.725124999999998</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
@@ -3773,10 +3755,10 @@
         <v>103</v>
       </c>
       <c r="M55" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="N55" s="1" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
@@ -3811,10 +3793,10 @@
         <v>103</v>
       </c>
       <c r="M56" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="N56" s="1" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.2">
@@ -3855,10 +3837,10 @@
         <v>103</v>
       </c>
       <c r="M57" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="N57" s="1" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.2">
@@ -3893,10 +3875,10 @@
         <v>103</v>
       </c>
       <c r="M58" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="N58" s="1" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.2">
@@ -3937,10 +3919,10 @@
         <v>103</v>
       </c>
       <c r="M59" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.2">
@@ -4025,10 +4007,10 @@
         <v>103</v>
       </c>
       <c r="M61" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="N61" s="1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.2">
@@ -4151,10 +4133,10 @@
         <v>103</v>
       </c>
       <c r="M64" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="N64" s="1" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
@@ -4239,10 +4221,10 @@
         <v>103</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="N66" s="1" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
@@ -4277,10 +4259,10 @@
         <v>103</v>
       </c>
       <c r="M67" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="N67" s="1" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
@@ -4315,10 +4297,10 @@
         <v>103</v>
       </c>
       <c r="M68" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="N68" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
@@ -4353,10 +4335,10 @@
         <v>103</v>
       </c>
       <c r="M69" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="N69" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
@@ -4435,10 +4417,10 @@
         <v>103</v>
       </c>
       <c r="M71" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="N71" s="1" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
@@ -4523,10 +4505,10 @@
         <v>103</v>
       </c>
       <c r="M73" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="N73" s="1" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
@@ -4605,10 +4587,10 @@
         <v>103</v>
       </c>
       <c r="M75" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="N75" s="1" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
@@ -4648,11 +4630,11 @@
       <c r="L76" t="s">
         <v>103</v>
       </c>
-      <c r="M76" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="N76" s="1" t="s">
-        <v>350</v>
+      <c r="M76" s="1">
+        <v>-37.813600000000001</v>
+      </c>
+      <c r="N76" s="1">
+        <v>144.9631</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
@@ -4731,10 +4713,10 @@
         <v>103</v>
       </c>
       <c r="M78" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="N78" s="1" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.2">
@@ -4769,10 +4751,10 @@
         <v>103</v>
       </c>
       <c r="M79" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="N79" s="1" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
@@ -4813,10 +4795,10 @@
         <v>103</v>
       </c>
       <c r="M80" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="N80" s="1" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
@@ -4857,10 +4839,10 @@
         <v>103</v>
       </c>
       <c r="M81" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="N81" s="1" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
@@ -4894,11 +4876,11 @@
       <c r="L82" t="s">
         <v>103</v>
       </c>
-      <c r="M82" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="N82" s="1" t="s">
-        <v>355</v>
+      <c r="M82" s="1">
+        <v>-31.416664999999998</v>
+      </c>
+      <c r="N82" s="1">
+        <v>-64.1833326</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
@@ -4933,10 +4915,10 @@
         <v>103</v>
       </c>
       <c r="M83" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="N83" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
@@ -4977,10 +4959,10 @@
         <v>103</v>
       </c>
       <c r="M84" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N84" s="1" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
@@ -5015,10 +4997,10 @@
         <v>103</v>
       </c>
       <c r="M85" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="N85" s="1" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
@@ -5053,10 +5035,10 @@
         <v>103</v>
       </c>
       <c r="M86" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="N86" s="1" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.2">
@@ -5091,10 +5073,10 @@
         <v>103</v>
       </c>
       <c r="M87" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="N87" s="1" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
@@ -5129,10 +5111,10 @@
         <v>103</v>
       </c>
       <c r="M88" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="N88" s="1" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
@@ -5167,10 +5149,10 @@
         <v>103</v>
       </c>
       <c r="M89" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="N89" s="1" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
@@ -5211,10 +5193,10 @@
         <v>103</v>
       </c>
       <c r="M90" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="N90" s="1" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
@@ -5258,7 +5240,7 @@
         <v>248</v>
       </c>
       <c r="N91" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
@@ -5302,7 +5284,7 @@
         <v>253</v>
       </c>
       <c r="N92" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
@@ -5390,7 +5372,7 @@
         <v>254</v>
       </c>
       <c r="N94" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.2">
@@ -5434,7 +5416,7 @@
         <v>259</v>
       </c>
       <c r="N95" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.2">
@@ -5472,7 +5454,7 @@
         <v>260</v>
       </c>
       <c r="N96" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.2">
@@ -5510,7 +5492,7 @@
         <v>261</v>
       </c>
       <c r="N97" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.2">
@@ -5554,7 +5536,7 @@
         <v>262</v>
       </c>
       <c r="N98" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.2">
@@ -5592,7 +5574,7 @@
         <v>263</v>
       </c>
       <c r="N99" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
@@ -5630,7 +5612,7 @@
         <v>264</v>
       </c>
       <c r="N100" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.2">
@@ -5668,7 +5650,7 @@
         <v>265</v>
       </c>
       <c r="N101" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
@@ -5706,7 +5688,7 @@
         <v>266</v>
       </c>
       <c r="N102" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
@@ -5794,7 +5776,7 @@
         <v>42.360100000000003</v>
       </c>
       <c r="N104" s="1">
-        <v>71.058899999999994</v>
+        <v>-71.058899999999994</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
@@ -5838,7 +5820,7 @@
         <v>267</v>
       </c>
       <c r="N105" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
@@ -5876,7 +5858,7 @@
         <v>268</v>
       </c>
       <c r="N106" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
@@ -5920,7 +5902,7 @@
         <v>269</v>
       </c>
       <c r="N107" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
@@ -5964,7 +5946,7 @@
         <v>41.878100000000003</v>
       </c>
       <c r="N108" s="2">
-        <v>87.629800000000003</v>
+        <v>-87.629800000000003</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.2">
@@ -6002,7 +5984,7 @@
         <v>270</v>
       </c>
       <c r="N109" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.2">
@@ -6040,7 +6022,7 @@
         <v>271</v>
       </c>
       <c r="N110" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.2">
@@ -6128,7 +6110,7 @@
         <v>272</v>
       </c>
       <c r="N112" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
@@ -6172,7 +6154,7 @@
         <v>273</v>
       </c>
       <c r="N113" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
@@ -6216,7 +6198,7 @@
         <v>274</v>
       </c>
       <c r="N114" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
@@ -6256,11 +6238,11 @@
       <c r="L115" t="s">
         <v>103</v>
       </c>
-      <c r="M115" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="N115" s="1" t="s">
-        <v>334</v>
+      <c r="M115" s="1">
+        <v>45.357315</v>
+      </c>
+      <c r="N115" s="1">
+        <v>36.468291999999998</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.2">
@@ -6294,11 +6276,11 @@
       <c r="L116" t="s">
         <v>103</v>
       </c>
-      <c r="M116" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="N116" s="1" t="s">
-        <v>335</v>
+      <c r="M116" s="1">
+        <v>37.995538000000003</v>
+      </c>
+      <c r="N116" s="1">
+        <v>23.725124999999998</v>
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.2">
@@ -6339,10 +6321,10 @@
         <v>103</v>
       </c>
       <c r="M117" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="N117" s="1" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.2">
@@ -6377,10 +6359,10 @@
         <v>103</v>
       </c>
       <c r="M118" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="N118" s="1" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.2">
@@ -6421,10 +6403,10 @@
         <v>103</v>
       </c>
       <c r="M119" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="N119" s="1" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.2">
@@ -6459,10 +6441,10 @@
         <v>103</v>
       </c>
       <c r="M120" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="N120" s="1" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.2">
@@ -6503,10 +6485,10 @@
         <v>103</v>
       </c>
       <c r="M121" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="N121" s="1" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.2">
@@ -6591,10 +6573,10 @@
         <v>103</v>
       </c>
       <c r="M123" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="N123" s="1" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.2">
@@ -6717,10 +6699,10 @@
         <v>103</v>
       </c>
       <c r="M126" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="N126" s="1" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.2">
@@ -6805,10 +6787,10 @@
         <v>103</v>
       </c>
       <c r="M128" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="N128" s="1" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
     </row>
     <row r="129" spans="1:14" x14ac:dyDescent="0.2">
@@ -6843,10 +6825,10 @@
         <v>103</v>
       </c>
       <c r="M129" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="N129" s="1" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
     </row>
     <row r="130" spans="1:14" x14ac:dyDescent="0.2">
@@ -6881,10 +6863,10 @@
         <v>103</v>
       </c>
       <c r="M130" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="N130" s="1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
     </row>
     <row r="131" spans="1:14" x14ac:dyDescent="0.2">
@@ -6919,10 +6901,10 @@
         <v>103</v>
       </c>
       <c r="M131" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="N131" s="1" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
     </row>
     <row r="132" spans="1:14" x14ac:dyDescent="0.2">
@@ -7001,10 +6983,10 @@
         <v>103</v>
       </c>
       <c r="M133" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="N133" s="1" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.2">
@@ -7089,10 +7071,10 @@
         <v>103</v>
       </c>
       <c r="M135" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="N135" s="1" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.2">
@@ -7171,10 +7153,10 @@
         <v>103</v>
       </c>
       <c r="M137" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="N137" s="1" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="138" spans="1:14" x14ac:dyDescent="0.2">
@@ -7214,11 +7196,11 @@
       <c r="L138" t="s">
         <v>103</v>
       </c>
-      <c r="M138" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="N138" s="1" t="s">
-        <v>350</v>
+      <c r="M138" s="1">
+        <v>-37.813600000000001</v>
+      </c>
+      <c r="N138" s="1">
+        <v>144.9631</v>
       </c>
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.2">
@@ -7297,10 +7279,10 @@
         <v>103</v>
       </c>
       <c r="M140" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="N140" s="1" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
     </row>
     <row r="141" spans="1:14" x14ac:dyDescent="0.2">
@@ -7335,10 +7317,10 @@
         <v>103</v>
       </c>
       <c r="M141" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="N141" s="1" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
     </row>
     <row r="142" spans="1:14" x14ac:dyDescent="0.2">
@@ -7379,10 +7361,10 @@
         <v>103</v>
       </c>
       <c r="M142" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="N142" s="1" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
     </row>
     <row r="143" spans="1:14" x14ac:dyDescent="0.2">
@@ -7423,10 +7405,10 @@
         <v>103</v>
       </c>
       <c r="M143" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="N143" s="1" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
     </row>
     <row r="144" spans="1:14" x14ac:dyDescent="0.2">
@@ -7461,10 +7443,10 @@
         <v>103</v>
       </c>
       <c r="M144" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="N144" s="1" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.2">
@@ -7499,10 +7481,10 @@
         <v>103</v>
       </c>
       <c r="M145" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="N145" s="1" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.2">
@@ -7543,10 +7525,10 @@
         <v>103</v>
       </c>
       <c r="M146" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="N146" s="1" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.2">
@@ -7581,10 +7563,10 @@
         <v>103</v>
       </c>
       <c r="M147" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="N147" s="1" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.2">
@@ -7619,10 +7601,10 @@
         <v>103</v>
       </c>
       <c r="M148" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="N148" s="1" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.2">
@@ -7657,10 +7639,10 @@
         <v>103</v>
       </c>
       <c r="M149" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="N149" s="1" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.2">
@@ -7695,10 +7677,10 @@
         <v>103</v>
       </c>
       <c r="M150" s="1" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="N150" s="1" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.2">
@@ -7733,10 +7715,10 @@
         <v>103</v>
       </c>
       <c r="M151" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="N151" s="1" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.2">
@@ -7777,10 +7759,10 @@
         <v>103</v>
       </c>
       <c r="M152" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="N152" s="1" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.2">
@@ -7815,10 +7797,10 @@
         <v>103</v>
       </c>
       <c r="M153" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="N153" s="1" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>